<commit_message>
Finished all indicators except for ones pertaining to country name, region, edf & edm 2015, and mobilebb
</commit_message>
<xml_diff>
--- a/IM-testing/[IM] Codebook.xlsx
+++ b/IM-testing/[IM] Codebook.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dylanhuang/Git/Ubuntu64/IM-testing/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dylanhuang/Ubuntu64/IM-testing/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -4787,7 +4787,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -4867,6 +4867,11 @@
       <color theme="4"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -4924,7 +4929,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -4996,6 +5001,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5436,6 +5445,159 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="9" name="Rectangle 1" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12700000" cy="12700000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>279400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="Rectangle 1" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12700000" cy="12700000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>279400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="Rectangle 1" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12700000" cy="12700000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>279400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="Rectangle 1" hidden="1"/>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -5935,6 +6097,159 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12700000" cy="12700000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12700000" cy="12700000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12700000" cy="12700000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -6204,10 +6519,10 @@
   <dimension ref="A1:Z1004"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C77" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A95" sqref="A95"/>
+      <selection pane="bottomRight" activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -6297,7 +6612,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="39" t="s">
         <v>1561</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -6337,7 +6652,7 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="37" t="s">
+      <c r="A6" s="39" t="s">
         <v>22</v>
       </c>
       <c r="B6" s="7" t="s">
@@ -6377,7 +6692,7 @@
       </c>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="37" t="s">
+      <c r="A8" s="39" t="s">
         <v>29</v>
       </c>
       <c r="B8" s="7" t="s">
@@ -6417,7 +6732,7 @@
       </c>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="37" t="s">
+      <c r="A10" s="39" t="s">
         <v>33</v>
       </c>
       <c r="B10" s="7" t="s">
@@ -6457,7 +6772,7 @@
       </c>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="37" t="s">
+      <c r="A12" s="39" t="s">
         <v>37</v>
       </c>
       <c r="B12" s="7" t="s">
@@ -6497,7 +6812,7 @@
       </c>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="37" t="s">
+      <c r="A14" s="39" t="s">
         <v>41</v>
       </c>
       <c r="B14" s="7" t="s">
@@ -6537,7 +6852,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="37" t="s">
+      <c r="A16" s="39" t="s">
         <v>45</v>
       </c>
       <c r="B16" s="7" t="s">
@@ -6577,7 +6892,7 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="37" t="s">
+      <c r="A18" s="39" t="s">
         <v>49</v>
       </c>
       <c r="B18" s="7" t="s">
@@ -6617,7 +6932,7 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="37" t="s">
+      <c r="A20" s="39" t="s">
         <v>53</v>
       </c>
       <c r="B20" s="7" t="s">
@@ -6657,7 +6972,7 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="37" t="s">
+      <c r="A22" s="39" t="s">
         <v>57</v>
       </c>
       <c r="B22" s="7" t="s">
@@ -6728,7 +7043,7 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="38" t="s">
+      <c r="A26" s="40" t="s">
         <v>65</v>
       </c>
       <c r="B26" s="4" t="s">
@@ -7493,7 +7808,7 @@
       </c>
     </row>
     <row r="65" spans="1:8" ht="13" x14ac:dyDescent="0.15">
-      <c r="A65" s="6" t="s">
+      <c r="A65" s="31" t="s">
         <v>164</v>
       </c>
       <c r="B65" s="4" t="s">
@@ -7510,7 +7825,7 @@
       </c>
     </row>
     <row r="66" spans="1:8" ht="13" x14ac:dyDescent="0.15">
-      <c r="A66" s="6" t="s">
+      <c r="A66" s="31" t="s">
         <v>167</v>
       </c>
       <c r="B66" s="4" t="s">
@@ -7524,7 +7839,7 @@
       </c>
     </row>
     <row r="67" spans="1:8" ht="13" x14ac:dyDescent="0.15">
-      <c r="A67" s="6" t="s">
+      <c r="A67" s="31" t="s">
         <v>169</v>
       </c>
       <c r="B67" s="4" t="s">
@@ -7538,7 +7853,7 @@
       </c>
     </row>
     <row r="68" spans="1:8" ht="13" x14ac:dyDescent="0.15">
-      <c r="A68" s="6" t="s">
+      <c r="A68" s="31" t="s">
         <v>171</v>
       </c>
       <c r="B68" s="4" t="s">
@@ -15244,7 +15559,7 @@
       </c>
     </row>
     <row r="498" spans="1:4" ht="13" x14ac:dyDescent="0.15">
-      <c r="A498" s="6" t="s">
+      <c r="A498" s="31" t="s">
         <v>1068</v>
       </c>
       <c r="B498" s="4" t="s">
@@ -15255,7 +15570,7 @@
       </c>
     </row>
     <row r="499" spans="1:4" ht="13" x14ac:dyDescent="0.15">
-      <c r="A499" s="6" t="s">
+      <c r="A499" s="31" t="s">
         <v>1070</v>
       </c>
       <c r="B499" s="4" t="s">
@@ -15266,31 +15581,31 @@
       </c>
     </row>
     <row r="500" spans="1:4" ht="13" x14ac:dyDescent="0.15">
-      <c r="A500" s="33" t="s">
+      <c r="A500" s="31" t="s">
         <v>1559</v>
       </c>
       <c r="B500" s="5"/>
     </row>
     <row r="501" spans="1:4" ht="13" x14ac:dyDescent="0.15">
-      <c r="A501" s="33" t="s">
+      <c r="A501" s="31" t="s">
         <v>1555</v>
       </c>
       <c r="B501" s="5"/>
     </row>
     <row r="502" spans="1:4" ht="13" x14ac:dyDescent="0.15">
-      <c r="A502" s="33" t="s">
+      <c r="A502" s="31" t="s">
         <v>1558</v>
       </c>
       <c r="B502" s="5"/>
     </row>
     <row r="503" spans="1:4" ht="13" x14ac:dyDescent="0.15">
-      <c r="A503" s="33" t="s">
+      <c r="A503" s="31" t="s">
         <v>1556</v>
       </c>
       <c r="B503" s="5"/>
     </row>
     <row r="504" spans="1:4" ht="13" x14ac:dyDescent="0.15">
-      <c r="A504" s="33" t="s">
+      <c r="A504" s="31" t="s">
         <v>1557</v>
       </c>
       <c r="B504" s="5"/>

</xml_diff>